<commit_message>
Complete sharing image features
</commit_message>
<xml_diff>
--- a/storage/import_data/service_data.xlsx
+++ b/storage/import_data/service_data.xlsx
@@ -11,9 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
-  <si>
-    <t>servizio</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>service</t>
   </si>
   <si>
     <t>desc</t>
@@ -37,22 +40,34 @@
     <t>gb</t>
   </si>
   <si>
+    <t>netflix</t>
+  </si>
+  <si>
     <t>Netflix</t>
   </si>
   <si>
     <t>Servizio streaming video Ultra HD</t>
   </si>
   <si>
+    <t>amazonmusic</t>
+  </si>
+  <si>
     <t>Amazon Music</t>
   </si>
   <si>
     <t xml:space="preserve">Servizio musica streaming </t>
   </si>
   <si>
+    <t>applemusic</t>
+  </si>
+  <si>
     <t>Apple Music</t>
   </si>
   <si>
     <t>Servizio musica streaming</t>
+  </si>
+  <si>
+    <t>spotifyfamily</t>
   </si>
   <si>
     <t>Spotify Family</t>
@@ -99,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -112,14 +127,17 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -337,160 +355,178 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="29.0"/>
+    <col customWidth="1" min="3" max="3" width="29.0"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="5">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="6">
         <v>4.0</v>
       </c>
-      <c r="E2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="F2" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G2" s="4">
         <v>17.99</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="4">
         <v>20.99</v>
       </c>
-      <c r="H2" s="6">
+      <c r="I2" s="4">
         <v>14.99</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="5">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="6">
         <v>6.0</v>
       </c>
-      <c r="E3" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="F3" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G3" s="4">
         <v>13.99</v>
       </c>
-      <c r="G3" s="6">
+      <c r="H3" s="4">
         <v>17.99</v>
       </c>
-      <c r="H3" s="6">
+      <c r="I3" s="4">
         <v>16.99</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="5">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="6">
         <v>3.0</v>
       </c>
-      <c r="E4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="F4" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G4" s="4">
         <v>15.99</v>
       </c>
-      <c r="G4" s="6">
+      <c r="H4" s="4">
         <v>18.99</v>
       </c>
-      <c r="H4" s="6">
+      <c r="I4" s="4">
         <v>15.99</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="5">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="7">
         <v>1.0</v>
       </c>
-      <c r="D5" s="5">
+      <c r="E5" s="6">
         <v>5.0</v>
       </c>
-      <c r="E5" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="F5" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="4">
         <v>14.99</v>
       </c>
-      <c r="G5" s="6">
+      <c r="H5" s="4">
         <v>16.99</v>
       </c>
-      <c r="H5" s="6">
+      <c r="I5" s="4">
         <v>12.99</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="D6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="E6" s="6">
         <v>10.0</v>
       </c>
-      <c r="E6" s="5">
+      <c r="F6" s="6">
         <v>1.0</v>
       </c>
-      <c r="F6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="G6" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="I6" s="4">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>